<commit_message>
fixed some typing issues
</commit_message>
<xml_diff>
--- a/data/users_conditional_styling.xlsx
+++ b/data/users_conditional_styling.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -32,9 +32,6 @@
     <t>alice.white@example.com</t>
   </si>
   <si>
-    <t>17</t>
-  </si>
-  <si>
     <t>Teen</t>
   </si>
   <si>
@@ -44,9 +41,6 @@
     <t>bob.brown@example.com</t>
   </si>
   <si>
-    <t>22</t>
-  </si>
-  <si>
     <t>Young Adult</t>
   </si>
   <si>
@@ -56,9 +50,6 @@
     <t>charlie.gray@example.com</t>
   </si>
   <si>
-    <t>31</t>
-  </si>
-  <si>
     <t>Adult</t>
   </si>
   <si>
@@ -68,45 +59,30 @@
     <t>diana.blue@example.com</t>
   </si>
   <si>
-    <t>45</t>
-  </si>
-  <si>
     <t>Ethan Black</t>
   </si>
   <si>
     <t>ethan.black@example.com</t>
   </si>
   <si>
-    <t>19</t>
-  </si>
-  <si>
     <t>Fiona Green</t>
   </si>
   <si>
     <t>fiona.green@example.com</t>
   </si>
   <si>
-    <t>28</t>
-  </si>
-  <si>
     <t>George Red</t>
   </si>
   <si>
     <t>george.red@example.com</t>
   </si>
   <si>
-    <t>33</t>
-  </si>
-  <si>
     <t>Hannah Silver</t>
   </si>
   <si>
     <t>hannah.silver@example.com</t>
   </si>
   <si>
-    <t>61</t>
-  </si>
-  <si>
     <t>Senior</t>
   </si>
   <si>
@@ -116,16 +92,10 @@
     <t>ian.gold@example.com</t>
   </si>
   <si>
-    <t>15</t>
-  </si>
-  <si>
     <t>Jenny Rose</t>
   </si>
   <si>
     <t>jenny.rose@example.com</t>
-  </si>
-  <si>
-    <t>65</t>
   </si>
 </sst>
 </file>
@@ -252,137 +222,137 @@
       <c r="B2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="n" s="0">
+        <v>17.0</v>
+      </c>
+      <c r="D2" t="s" s="2">
         <v>6</v>
-      </c>
-      <c r="D2" t="s" s="2">
-        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="C3" t="n" s="0">
+        <v>22.0</v>
+      </c>
+      <c r="D3" t="s" s="3">
         <v>9</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s" s="3">
-        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C4" t="n" s="0">
+        <v>31.0</v>
+      </c>
+      <c r="D4" t="s" s="4">
         <v>12</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s" s="4">
-        <v>15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>18</v>
+        <v>14</v>
+      </c>
+      <c r="C5" t="n" s="0">
+        <v>45.0</v>
       </c>
       <c r="D5" t="s" s="5">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>21</v>
+        <v>16</v>
+      </c>
+      <c r="C6" t="n" s="0">
+        <v>19.0</v>
       </c>
       <c r="D6" t="s" s="6">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>24</v>
+        <v>18</v>
+      </c>
+      <c r="C7" t="n" s="0">
+        <v>28.0</v>
       </c>
       <c r="D7" t="s" s="7">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>27</v>
+        <v>20</v>
+      </c>
+      <c r="C8" t="n" s="0">
+        <v>33.0</v>
       </c>
       <c r="D8" t="s" s="8">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s" s="0">
-        <v>30</v>
+        <v>22</v>
+      </c>
+      <c r="C9" t="n" s="0">
+        <v>61.0</v>
       </c>
       <c r="D9" t="s" s="9">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="C10" t="s" s="0">
-        <v>34</v>
+        <v>25</v>
+      </c>
+      <c r="C10" t="n" s="0">
+        <v>15.0</v>
       </c>
       <c r="D10" t="s" s="10">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="C11" t="s" s="0">
-        <v>37</v>
+        <v>27</v>
+      </c>
+      <c r="C11" t="n" s="0">
+        <v>65.0</v>
       </c>
       <c r="D11" t="s" s="11">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>